<commit_message>
admin home page added
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -190,6 +190,18 @@
   </si>
   <si>
     <t>∞</t>
+  </si>
+  <si>
+    <t>commits are not much but are valuable and tested</t>
+  </si>
+  <si>
+    <t>yavor2000</t>
+  </si>
+  <si>
+    <t>Явор Митев</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -648,7 +660,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -658,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +707,9 @@
       <c r="B4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
@@ -703,7 +717,9 @@
       <c r="B5" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
@@ -728,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
@@ -740,12 +756,14 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B10" s="13" t="s">
@@ -939,7 +957,9 @@
       <c r="B26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>10</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>3</v>
       </c>
@@ -949,7 +969,9 @@
       <c r="B27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
       </c>
@@ -971,7 +993,9 @@
       <c r="B29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="5"/>
+      <c r="C29" s="5">
+        <v>5</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>5</v>
       </c>
@@ -981,7 +1005,9 @@
       <c r="B30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="5">
+        <v>5</v>
+      </c>
       <c r="D30" s="5" t="s">
         <v>5</v>
       </c>
@@ -1023,7 +1049,9 @@
       <c r="B34" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D34" s="7" t="s">
         <v>28</v>
       </c>
@@ -1195,7 +1223,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>205</v>
+        <v>161</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>